<commit_message>
Add dynamic description w/ tests
</commit_message>
<xml_diff>
--- a/etc/content.xlsx
+++ b/etc/content.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\git\pods\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmenedes\git\pods\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54247D69-9AE3-431B-A91E-20F3FACBD916}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="content" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>key</t>
   </si>
@@ -49,19 +48,25 @@
     <t>pods_url</t>
   </si>
   <si>
-    <t>Please use the NYC Health Logo to refresh the map and return to the full list of facilities.</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>https://services3.arcgis.com/A6Zjpzrub8ESZ3c7/arcgis/rest/services/vwLatestDateLocator/FeatureServer/0/query?f=pgeojson&amp;outSR=2263&amp;outFields=ActivePOD%20as%20activepod,DOHMHPODLink%20as%20lnk,DOECode%20as%20id,PODSiteName%20as%20name,Address%20as%20addr,Borough%20as%20boro,ZIP%20as%20zip,Ops_status%20as%20status,OpeningTime%20as%20opening,wait_time%20as%20wait,LatestDate%20as%20updated,%20LabelPos%20as%20labelpos&amp;where=activepod%3D1</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;No POD activation is currently in place.&lt;/h2&gt;&lt;p&gt;Points of Dispensing (PODs) are temporary sites that are ready to open to provide life-saving medications to anyone who needs them after a biological attack or during a communicable disease outbreak. The sites are located throughout the city and are run by the NYC Department of Health and Mental Hygiene. All NYC POD sites are wheelchair accessible. For more information, please visit our &lt;a href=https://www1.nyc.gov/site/doh/health/emergency-preparedness/emergency-medication-distribution.page&gt;webpage.&lt;/a&gt;&lt;br&gt;&lt;br&gt;If you do not live in NYC, please check with your local health department:  &lt;a href=http://www.nassaucountyny.gov/agencies/Health/index.html&gt;Nassau County&lt;/a&gt;, &lt;a href=https://www.suffolkcountyny.gov/health&gt;Suffolk County&lt;/a&gt;, &lt;a href=https://www.co.bergen.nj.us/departments-and-services/about-health-services&gt;Bergen County&lt;/a&gt;, &lt;a href=https://www.health.ny.gov/contact/contact_information&gt;New York State&lt;/a&gt;, &lt;a href=https://www.state.nj.us/health/lh/community&gt; New Jersey State&lt;/a&gt;.&lt;/p&gt;&amp;quot;</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Not all Points of Dispensing sites may be activated at the time of an event. Please continue checking this page to see which sites are activated following an event. If you do not live in NYC, please check with your local health department.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -903,11 +908,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -949,7 +954,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,17 +962,25 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/FZPEZdE6NbEJ3iYRc9P1xZvbBFVZmyZohI6xWWZDcAJjySdvuQEnJ78VunDg2D4i9RLh/SKGEqzuAWqmzzWRQ==" saltValue="SapJTy4q4w8G4Qy6VNbWhg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="JBELkc9A0bXkONC+CoUbCQy/8Z1jQCemyVDtbBgRc/O0FWuJA+1dDeDGom9I1cLjUt3aEHdEte8tyFi9GQp/5w==" saltValue="wQaTZEKspZMt62J4lzgABg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Value must be true or false - select from dropdown" sqref="B5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Value must be true or false - select from dropdown" sqref="B5">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>